<commit_message>
Add header in output. Fix non integer parity bug.
</commit_message>
<xml_diff>
--- a/test/reader/dong_ying/waste.xlsx
+++ b/test/reader/dong_ying/waste.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,79 +452,84 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>185403</v>
+          <t>Breed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>有問題</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="n">
-        <v>44609</v>
+          <t>confusing_note</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Birthday</t>
+        </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Y121005地</t>
+          <t>Sire</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Y146101趙</t>
-        </is>
-      </c>
-      <c r="G1" t="n">
-        <v>244310</v>
+          <t>Dam</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>reg_id</t>
+        </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>地趙</t>
+          <t>Chinese_name</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>母</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>['不允許有相近耳號']</t>
+          <t>Gender</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>188003</v>
+        <v>185403</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>L?</t>
+          <t>有問題</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>44665</v>
-      </c>
-      <c r="E2" t="n">
-        <v/>
-      </c>
-      <c r="F2" t="n">
-        <v/>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>無登</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v/>
+        <v>44609</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Y121005地</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Y146101趙</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>244310</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>地趙</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -543,34 +548,30 @@
           <t>L</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>190202</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3" s="1" t="n">
+        <v>188003</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>L?</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>44665</v>
+      </c>
+      <c r="E3" t="n">
         <v/>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>44705</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Y155009合</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Y126104地</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>????</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>????</t>
-        </is>
+      <c r="F3" t="n">
+        <v/>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>無登</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v/>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -579,47 +580,93 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['登錄號不能含有非數字字元 ']</t>
+          <t>['不允許有相近耳號']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>190202</v>
+      </c>
+      <c r="C4" t="n">
+        <v/>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>44705</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Y155009合</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Y126104地</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>母</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>['登錄號不能含有非數字字元 ']</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B5" s="1" t="n">
         <v>137105</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>137108</v>
       </c>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" t="inlineStr">
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>Y195207王</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Y182001趙</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="G5" t="n">
         <v>238789</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>王趙</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>母</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>['不允許有相近耳號']</t>
         </is>

</xml_diff>